<commit_message>
This is a new updated file
</commit_message>
<xml_diff>
--- a/OCB Weekly Health Report (14th-20th)July 2018 .xlsx
+++ b/OCB Weekly Health Report (14th-20th)July 2018 .xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="234">
   <si>
     <t>Server Name</t>
   </si>
@@ -715,6 +715,9 @@
   </si>
   <si>
     <t>16.8ddd</t>
+  </si>
+  <si>
+    <t>90000new</t>
   </si>
 </sst>
 </file>
@@ -1086,6 +1089,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1109,9 +1115,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1418,7 +1421,7 @@
   <dimension ref="A1:Z79"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1465,17 +1468,17 @@
       <c r="J3" s="10"/>
     </row>
     <row r="4" spans="1:26" s="2" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="51" t="s">
         <v>231</v>
       </c>
-      <c r="B4" s="50"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50"/>
-      <c r="I4" s="50"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
       <c r="J4" s="10"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
@@ -1495,34 +1498,34 @@
       <c r="Z4" s="1"/>
     </row>
     <row r="5" spans="1:26" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="52" t="s">
         <v>105</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="53" t="s">
+      <c r="C5" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="54" t="s">
+      <c r="D5" s="55" t="s">
         <v>68</v>
       </c>
-      <c r="E5" s="54"/>
-      <c r="F5" s="55" t="s">
+      <c r="E5" s="55"/>
+      <c r="F5" s="56" t="s">
         <v>98</v>
       </c>
-      <c r="G5" s="55"/>
-      <c r="H5" s="56" t="s">
+      <c r="G5" s="56"/>
+      <c r="H5" s="57" t="s">
         <v>99</v>
       </c>
-      <c r="I5" s="57"/>
+      <c r="I5" s="58"/>
     </row>
     <row r="6" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="52" t="s">
+      <c r="A6" s="53" t="s">
         <v>105</v>
       </c>
-      <c r="B6" s="52"/>
-      <c r="C6" s="53"/>
+      <c r="B6" s="53"/>
+      <c r="C6" s="54"/>
       <c r="D6" s="15" t="s">
         <v>72</v>
       </c>
@@ -1558,8 +1561,8 @@
       <c r="E7" s="8">
         <v>0.36</v>
       </c>
-      <c r="F7" s="8">
-        <v>90</v>
+      <c r="F7" s="8" t="s">
+        <v>233</v>
       </c>
       <c r="G7" s="46" t="s">
         <v>110</v>
@@ -1622,7 +1625,7 @@
       <c r="G9" s="46" t="s">
         <v>114</v>
       </c>
-      <c r="H9" s="58" t="s">
+      <c r="H9" s="50" t="s">
         <v>232</v>
       </c>
       <c r="I9" s="46" t="s">
@@ -3505,30 +3508,30 @@
       <c r="G2" s="11"/>
     </row>
     <row r="3" spans="4:9" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D3" s="50" t="s">
+      <c r="D3" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
     </row>
     <row r="4" spans="4:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50"/>
-      <c r="I4" s="50"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
     </row>
     <row r="5" spans="4:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="51"/>
     </row>
     <row r="6" spans="4:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E6" s="11"/>
@@ -3606,30 +3609,30 @@
       <c r="G20" s="11"/>
     </row>
     <row r="21" spans="4:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="D21" s="50" t="s">
+      <c r="D21" s="51" t="s">
         <v>66</v>
       </c>
-      <c r="E21" s="50"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="50"/>
-      <c r="H21" s="50"/>
-      <c r="I21" s="50"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="51"/>
+      <c r="I21" s="51"/>
     </row>
     <row r="22" spans="4:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="D22" s="50"/>
-      <c r="E22" s="50"/>
-      <c r="F22" s="50"/>
-      <c r="G22" s="50"/>
-      <c r="H22" s="50"/>
-      <c r="I22" s="50"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="51"/>
+      <c r="F22" s="51"/>
+      <c r="G22" s="51"/>
+      <c r="H22" s="51"/>
+      <c r="I22" s="51"/>
     </row>
     <row r="23" spans="4:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="D23" s="50"/>
-      <c r="E23" s="50"/>
-      <c r="F23" s="50"/>
-      <c r="G23" s="50"/>
-      <c r="H23" s="50"/>
-      <c r="I23" s="50"/>
+      <c r="D23" s="51"/>
+      <c r="E23" s="51"/>
+      <c r="F23" s="51"/>
+      <c r="G23" s="51"/>
+      <c r="H23" s="51"/>
+      <c r="I23" s="51"/>
     </row>
     <row r="24" spans="4:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="E24" s="11"/>

</xml_diff>